<commit_message>
firs commit branch testBranch
</commit_message>
<xml_diff>
--- a/账号管理.xlsx
+++ b/账号管理.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="SCP" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="394">
   <si>
     <t>121.199.31.234</t>
   </si>
@@ -2665,6 +2665,114 @@
   <si>
     <t>修改爵位等级</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>联合创始分红比例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>810</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>和</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>279</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>改成</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>85%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>改为</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>89%</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fxx.xinykj.com/pay/wxpay2/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>123456789123456789qwertyuioplkjh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商城后台管理：</t>
+  </si>
+  <si>
+    <t>账号：爱艾灸</t>
+  </si>
+  <si>
+    <t>密码：123456</t>
+  </si>
+  <si>
+    <t>微信公众</t>
+  </si>
+  <si>
+    <t>账号：</t>
+  </si>
+  <si>
+    <t>137845659@qq.com</t>
+  </si>
+  <si>
+    <t>密码：</t>
+  </si>
+  <si>
+    <t>aajp70093636</t>
+  </si>
+  <si>
+    <t>微信商户号：</t>
+  </si>
+  <si>
+    <t>账号：1245556702@1245556702</t>
+  </si>
+  <si>
+    <t>密码：093636</t>
   </si>
 </sst>
 </file>
@@ -3183,18 +3291,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3206,9 +3317,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4280,7 +4388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A11:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="E19" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
@@ -4383,7 +4491,7 @@
       <c r="D29" t="s">
         <v>326</v>
       </c>
-      <c r="E29" s="84" t="s">
+      <c r="E29" s="76" t="s">
         <v>378</v>
       </c>
     </row>
@@ -4397,7 +4505,7 @@
       <c r="D30" t="s">
         <v>329</v>
       </c>
-      <c r="E30" s="84" t="s">
+      <c r="E30" s="76" t="s">
         <v>378</v>
       </c>
     </row>
@@ -4445,7 +4553,7 @@
       <c r="D36" t="s">
         <v>324</v>
       </c>
-      <c r="E36" s="84" t="s">
+      <c r="E36" s="76" t="s">
         <v>378</v>
       </c>
     </row>
@@ -4492,10 +4600,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B7:C15"/>
+  <dimension ref="B7:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4531,10 +4639,64 @@
       <c r="B14" t="s">
         <v>371</v>
       </c>
+      <c r="C14" s="3">
+        <v>123</v>
+      </c>
     </row>
     <row r="15" spans="2:3">
       <c r="B15" t="s">
         <v>372</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" t="s">
+        <v>387</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" t="s">
+        <v>389</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" t="s">
+        <v>393</v>
       </c>
     </row>
   </sheetData>
@@ -4543,6 +4705,7 @@
     <hyperlink ref="C7" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4551,7 +4714,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4782,7 +4945,7 @@
         <v>286</v>
       </c>
       <c r="E15" t="s">
-        <v>245</v>
+        <v>381</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -4842,8 +5005,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46:F49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -5549,11 +5712,23 @@
     </row>
     <row r="42" spans="1:13" ht="14.25">
       <c r="A42" s="77"/>
-      <c r="B42" s="21"/>
-      <c r="C42" s="57"/>
-      <c r="D42" s="66"/>
+      <c r="B42" s="21" t="s">
+        <v>379</v>
+      </c>
+      <c r="C42" s="57" t="s">
+        <v>380</v>
+      </c>
+      <c r="D42" s="66">
+        <v>42563</v>
+      </c>
+      <c r="E42" t="s">
+        <v>242</v>
+      </c>
       <c r="F42" s="67"/>
       <c r="G42" s="67"/>
+      <c r="H42" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="43" spans="1:13" ht="93.75" hidden="1" customHeight="1">
       <c r="A43" s="77"/>
@@ -5633,14 +5808,14 @@
       <c r="C46" s="78" t="s">
         <v>294</v>
       </c>
-      <c r="D46" s="76">
+      <c r="D46" s="80">
         <v>42544</v>
       </c>
       <c r="E46" t="s">
         <v>242</v>
       </c>
-      <c r="F46" s="76"/>
-      <c r="G46" s="76">
+      <c r="F46" s="80"/>
+      <c r="G46" s="80">
         <v>42544</v>
       </c>
       <c r="H46" s="77" t="s">
@@ -5663,12 +5838,12 @@
       <c r="A47" s="77"/>
       <c r="B47" s="79"/>
       <c r="C47" s="78"/>
-      <c r="D47" s="76"/>
+      <c r="D47" s="80"/>
       <c r="E47" s="77" t="s">
         <v>242</v>
       </c>
-      <c r="F47" s="76"/>
-      <c r="G47" s="76"/>
+      <c r="F47" s="80"/>
+      <c r="G47" s="80"/>
       <c r="H47" s="77"/>
       <c r="I47" s="3">
         <v>802.86</v>
@@ -5684,10 +5859,10 @@
       <c r="A48" s="77"/>
       <c r="B48" s="79"/>
       <c r="C48" s="78"/>
-      <c r="D48" s="76"/>
+      <c r="D48" s="80"/>
       <c r="E48" s="77"/>
-      <c r="F48" s="76"/>
-      <c r="G48" s="76"/>
+      <c r="F48" s="80"/>
+      <c r="G48" s="80"/>
       <c r="H48" s="77"/>
       <c r="I48" s="3">
         <v>802.86</v>
@@ -5703,10 +5878,10 @@
       <c r="A49" s="77"/>
       <c r="B49" s="79"/>
       <c r="C49" s="78"/>
-      <c r="D49" s="76"/>
+      <c r="D49" s="80"/>
       <c r="E49" s="77"/>
-      <c r="F49" s="76"/>
-      <c r="G49" s="76"/>
+      <c r="F49" s="80"/>
+      <c r="G49" s="80"/>
       <c r="H49" s="77"/>
       <c r="I49" s="3">
         <v>3989</v>
@@ -5971,17 +6146,17 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="11">
+    <mergeCell ref="D46:D49"/>
+    <mergeCell ref="F46:F49"/>
+    <mergeCell ref="G46:G49"/>
+    <mergeCell ref="H46:H49"/>
+    <mergeCell ref="E47:E49"/>
     <mergeCell ref="A62:A80"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="A7:A49"/>
     <mergeCell ref="C46:C49"/>
     <mergeCell ref="B46:B49"/>
-    <mergeCell ref="D46:D49"/>
-    <mergeCell ref="F46:F49"/>
-    <mergeCell ref="G46:G49"/>
-    <mergeCell ref="H46:H49"/>
-    <mergeCell ref="E47:E49"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
@@ -6151,7 +6326,7 @@
       <c r="K1" s="10"/>
     </row>
     <row r="2" spans="1:11" ht="27">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="81" t="s">
         <v>86</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -6179,7 +6354,7 @@
       <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:11" ht="81">
-      <c r="A3" s="80"/>
+      <c r="A3" s="81"/>
       <c r="B3" s="8" t="s">
         <v>52</v>
       </c>
@@ -6205,7 +6380,7 @@
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:11" ht="27">
-      <c r="A4" s="80"/>
+      <c r="A4" s="81"/>
       <c r="B4" s="8" t="s">
         <v>67</v>
       </c>
@@ -6231,7 +6406,7 @@
       <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:11" ht="27">
-      <c r="A5" s="80"/>
+      <c r="A5" s="81"/>
       <c r="B5" s="8" t="s">
         <v>68</v>
       </c>
@@ -6257,7 +6432,7 @@
       <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="80"/>
+      <c r="A6" s="81"/>
       <c r="B6" s="8" t="s">
         <v>70</v>
       </c>
@@ -6283,7 +6458,7 @@
       <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:11" ht="67.5">
-      <c r="A7" s="80"/>
+      <c r="A7" s="81"/>
       <c r="B7" s="8"/>
       <c r="C7" s="9" t="s">
         <v>72</v>
@@ -6307,7 +6482,7 @@
       <c r="J7" s="8"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="80"/>
+      <c r="A8" s="81"/>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>73</v>
@@ -6331,7 +6506,7 @@
       <c r="J8" s="8"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="80"/>
+      <c r="A9" s="81"/>
       <c r="B9" s="8"/>
       <c r="C9" s="9"/>
       <c r="D9" s="13"/>
@@ -6343,7 +6518,7 @@
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="80"/>
+      <c r="A10" s="81"/>
       <c r="B10" s="8" t="s">
         <v>335</v>
       </c>
@@ -6361,7 +6536,7 @@
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="80"/>
+      <c r="A11" s="81"/>
       <c r="B11" s="8"/>
       <c r="C11" s="9"/>
       <c r="D11" s="13"/>
@@ -6373,7 +6548,7 @@
       <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="80"/>
+      <c r="A12" s="81"/>
       <c r="B12" s="8"/>
       <c r="C12" s="9"/>
       <c r="D12" s="13"/>
@@ -6385,12 +6560,12 @@
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="80"/>
+      <c r="A13" s="81"/>
       <c r="B13" s="8"/>
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="81" t="s">
+      <c r="A14" s="82" t="s">
         <v>198</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -6414,7 +6589,7 @@
       <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="82"/>
+      <c r="A15" s="83"/>
       <c r="B15" s="8" t="s">
         <v>201</v>
       </c>
@@ -6436,7 +6611,7 @@
       <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="82"/>
+      <c r="A16" s="83"/>
       <c r="B16" s="8" t="s">
         <v>200</v>
       </c>
@@ -6458,7 +6633,7 @@
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="82"/>
+      <c r="A17" s="83"/>
       <c r="B17" s="8" t="s">
         <v>202</v>
       </c>
@@ -6480,7 +6655,7 @@
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="82"/>
+      <c r="A18" s="83"/>
       <c r="B18" s="8" t="s">
         <v>203</v>
       </c>
@@ -6502,7 +6677,7 @@
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="83"/>
+      <c r="A19" s="84"/>
       <c r="B19" s="8" t="s">
         <v>204</v>
       </c>
@@ -7222,10 +7397,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R46"/>
+  <dimension ref="A1:R299"/>
   <sheetViews>
-    <sheetView topLeftCell="A247" workbookViewId="0">
-      <selection activeCell="S37" sqref="S37"/>
+    <sheetView topLeftCell="A266" workbookViewId="0">
+      <selection activeCell="P272" sqref="P272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -7246,6 +7421,26 @@
     <row r="46" spans="18:18">
       <c r="R46" t="s">
         <v>367</v>
+      </c>
+    </row>
+    <row r="263" spans="16:17">
+      <c r="Q263" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="272" spans="16:17">
+      <c r="P272" t="e">
+        <f>len</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="Q272" t="e">
+        <f>len</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="299" spans="9:9">
+      <c r="I299" t="s">
+        <v>382</v>
       </c>
     </row>
   </sheetData>

</xml_diff>